<commit_message>
edit project-outline file (for reviews resource and API docs)
</commit_message>
<xml_diff>
--- a/document/phan-cong-cong-viec.xlsx
+++ b/document/phan-cong-cong-viec.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84367\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\super-tours\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7B4F32-B927-470D-B2E3-2E83E4A0A8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,10 +180,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -843,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -913,6 +913,103 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
@@ -923,128 +1020,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,7 +1098,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Oval 2"/>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1158,7 +1158,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Oval 9"/>
+        <xdr:cNvPr id="10" name="Oval 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1212,7 +1218,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Oval 10"/>
+        <xdr:cNvPr id="11" name="Oval 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1266,7 +1278,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Oval 11"/>
+        <xdr:cNvPr id="12" name="Oval 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1320,7 +1338,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Oval 20"/>
+        <xdr:cNvPr id="21" name="Oval 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1374,7 +1398,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Oval 21"/>
+        <xdr:cNvPr id="22" name="Oval 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1428,7 +1458,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Oval 22"/>
+        <xdr:cNvPr id="23" name="Oval 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1482,7 +1518,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Oval 23"/>
+        <xdr:cNvPr id="24" name="Oval 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1536,7 +1578,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Oval 24"/>
+        <xdr:cNvPr id="25" name="Oval 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1590,7 +1638,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Oval 25"/>
+        <xdr:cNvPr id="26" name="Oval 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1644,7 +1698,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Oval 26"/>
+        <xdr:cNvPr id="27" name="Oval 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1698,7 +1758,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Oval 27"/>
+        <xdr:cNvPr id="28" name="Oval 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1752,7 +1818,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Oval 29"/>
+        <xdr:cNvPr id="30" name="Oval 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1806,7 +1878,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Oval 31"/>
+        <xdr:cNvPr id="32" name="Oval 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1860,7 +1938,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Oval 33"/>
+        <xdr:cNvPr id="34" name="Oval 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1914,7 +1998,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="Oval 36"/>
+        <xdr:cNvPr id="37" name="Oval 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1968,7 +2058,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Oval 38"/>
+        <xdr:cNvPr id="39" name="Oval 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2022,7 +2118,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Oval 39"/>
+        <xdr:cNvPr id="40" name="Oval 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2076,7 +2178,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Oval 40"/>
+        <xdr:cNvPr id="41" name="Oval 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2130,7 +2238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="Oval 42"/>
+        <xdr:cNvPr id="43" name="Oval 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2184,7 +2298,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="Oval 44"/>
+        <xdr:cNvPr id="45" name="Oval 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2238,7 +2358,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Oval 45"/>
+        <xdr:cNvPr id="46" name="Oval 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2300,7 +2426,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Oval 46"/>
+        <xdr:cNvPr id="47" name="Oval 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2362,7 +2494,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Oval 47"/>
+        <xdr:cNvPr id="48" name="Oval 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2424,7 +2562,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Oval 48"/>
+        <xdr:cNvPr id="49" name="Oval 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2736,35 +2880,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="15" width="8.7109375" style="1" customWidth="1"/>
-    <col min="16" max="19" width="5.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="14.42578125" style="1"/>
+    <col min="1" max="1" width="3.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
+    <col min="7" max="15" width="8.6640625" style="1" customWidth="1"/>
+    <col min="16" max="19" width="5.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
       <c r="G1" s="26"/>
     </row>
     <row r="2" spans="2:19" ht="21" customHeight="1" thickBot="1">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2772,7 +2916,7 @@
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="74"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -2781,54 +2925,54 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="75" t="s">
+      <c r="P2" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="77"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="47"/>
     </row>
     <row r="3" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="46"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="51"/>
     </row>
     <row r="4" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="49"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="54"/>
     </row>
     <row r="5" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
       <c r="B5" s="57" t="s">
@@ -2857,52 +3001,52 @@
       <c r="S5" s="59"/>
     </row>
     <row r="6" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B6" s="66"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="61"/>
       <c r="D6" s="61"/>
       <c r="E6" s="62"/>
       <c r="F6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="63" t="s">
+      <c r="G6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="63" t="s">
+      <c r="I6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="63" t="s">
+      <c r="J6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="63" t="s">
+      <c r="K6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="63" t="s">
+      <c r="L6" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="63" t="s">
+      <c r="M6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="27" t="s">
         <v>25</v>
       </c>
       <c r="O6" s="24"/>
-      <c r="P6" s="60"/>
+      <c r="P6" s="63"/>
       <c r="Q6" s="61"/>
       <c r="R6" s="61"/>
       <c r="S6" s="62"/>
     </row>
     <row r="7" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B7" s="78">
+      <c r="B7" s="34">
         <v>1</v>
       </c>
       <c r="C7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -2916,25 +3060,25 @@
       <c r="P7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q7" s="69" t="s">
+      <c r="Q7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="69" t="s">
+      <c r="R7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="70" t="s">
+      <c r="S7" s="29" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B8" s="79">
+      <c r="B8" s="35">
         <v>2</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
@@ -2953,14 +3097,14 @@
       <c r="S8" s="14"/>
     </row>
     <row r="9" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B9" s="79">
+      <c r="B9" s="35">
         <v>3</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="9"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15"/>
@@ -2972,25 +3116,25 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
       <c r="P9" s="12"/>
-      <c r="Q9" s="71" t="s">
+      <c r="Q9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="71" t="s">
+      <c r="R9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="72" t="s">
+      <c r="S9" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B10" s="79">
+      <c r="B10" s="35">
         <v>4</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="9"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -3001,7 +3145,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="73" t="s">
+      <c r="P10" s="32" t="s">
         <v>4</v>
       </c>
       <c r="Q10" s="13"/>
@@ -3009,14 +3153,14 @@
       <c r="S10" s="14"/>
     </row>
     <row r="11" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B11" s="79">
+      <c r="B11" s="35">
         <v>5</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="9"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -3027,7 +3171,7 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="73" t="s">
+      <c r="P11" s="32" t="s">
         <v>4</v>
       </c>
       <c r="Q11" s="13"/>
@@ -3035,14 +3179,14 @@
       <c r="S11" s="14"/>
     </row>
     <row r="12" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B12" s="79">
+      <c r="B12" s="35">
         <v>6</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="9"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -3054,21 +3198,21 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
       <c r="P12" s="12"/>
-      <c r="Q12" s="71" t="s">
+      <c r="Q12" s="30" t="s">
         <v>4</v>
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="14"/>
     </row>
     <row r="13" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B13" s="79">
+      <c r="B13" s="35">
         <v>7</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="9"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -3082,19 +3226,19 @@
       <c r="P13" s="12"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
-      <c r="S13" s="72" t="s">
+      <c r="S13" s="31" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B14" s="79">
+      <c r="B14" s="35">
         <v>8</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -3107,20 +3251,20 @@
       <c r="O14" s="11"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="71" t="s">
+      <c r="R14" s="30" t="s">
         <v>4</v>
       </c>
       <c r="S14" s="14"/>
     </row>
     <row r="15" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B15" s="79">
+      <c r="B15" s="35">
         <v>9</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -3132,21 +3276,21 @@
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
       <c r="P15" s="12"/>
-      <c r="Q15" s="71" t="s">
+      <c r="Q15" s="30" t="s">
         <v>4</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B16" s="79">
+      <c r="B16" s="35">
         <v>10</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -3159,20 +3303,20 @@
       <c r="O16" s="11"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="71" t="s">
+      <c r="R16" s="30" t="s">
         <v>4</v>
       </c>
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B17" s="79">
+      <c r="B17" s="35">
         <v>11</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="9"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -3183,7 +3327,7 @@
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="73" t="s">
+      <c r="P17" s="32" t="s">
         <v>4</v>
       </c>
       <c r="Q17" s="13"/>
@@ -3191,14 +3335,14 @@
       <c r="S17" s="14"/>
     </row>
     <row r="18" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B18" s="79">
+      <c r="B18" s="35">
         <v>12</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="9"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
@@ -3209,7 +3353,7 @@
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="73" t="s">
+      <c r="P18" s="32" t="s">
         <v>4</v>
       </c>
       <c r="Q18" s="13"/>
@@ -3217,14 +3361,14 @@
       <c r="S18" s="14"/>
     </row>
     <row r="19" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B19" s="79">
+      <c r="B19" s="35">
         <v>13</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="9"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -3237,20 +3381,20 @@
       <c r="O19" s="11"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="71" t="s">
+      <c r="R19" s="30" t="s">
         <v>4</v>
       </c>
       <c r="S19" s="14"/>
     </row>
     <row r="20" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B20" s="79">
+      <c r="B20" s="35">
         <v>14</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="9"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -3262,21 +3406,21 @@
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="71" t="s">
+      <c r="Q20" s="30" t="s">
         <v>4</v>
       </c>
       <c r="R20" s="13"/>
       <c r="S20" s="14"/>
     </row>
     <row r="21" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B21" s="79">
+      <c r="B21" s="35">
         <v>15</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="9"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3290,19 +3434,19 @@
       <c r="P21" s="12"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
-      <c r="S21" s="72" t="s">
+      <c r="S21" s="31" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B22" s="79">
+      <c r="B22" s="35">
         <v>16</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="9"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -3313,7 +3457,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
-      <c r="P22" s="73" t="s">
+      <c r="P22" s="32" t="s">
         <v>4</v>
       </c>
       <c r="Q22" s="13"/>
@@ -3321,14 +3465,14 @@
       <c r="S22" s="14"/>
     </row>
     <row r="23" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B23" s="79">
+      <c r="B23" s="35">
         <v>17</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="9"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3339,7 +3483,7 @@
       <c r="M23" s="11"/>
       <c r="N23" s="18"/>
       <c r="O23" s="11"/>
-      <c r="P23" s="73" t="s">
+      <c r="P23" s="32" t="s">
         <v>4</v>
       </c>
       <c r="Q23" s="13"/>
@@ -3347,14 +3491,14 @@
       <c r="S23" s="14"/>
     </row>
     <row r="24" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B24" s="79">
+      <c r="B24" s="35">
         <v>18</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="9"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -3365,28 +3509,28 @@
       <c r="M24" s="11"/>
       <c r="N24" s="18"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="73" t="s">
+      <c r="P24" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="Q24" s="71" t="s">
+      <c r="Q24" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R24" s="71" t="s">
+      <c r="R24" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="S24" s="72" t="s">
+      <c r="S24" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B25" s="79">
+      <c r="B25" s="35">
         <v>19</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="9"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -3397,28 +3541,28 @@
       <c r="M25" s="11"/>
       <c r="N25" s="18"/>
       <c r="O25" s="11"/>
-      <c r="P25" s="73" t="s">
+      <c r="P25" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="Q25" s="71" t="s">
+      <c r="Q25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R25" s="71" t="s">
+      <c r="R25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="S25" s="72" t="s">
+      <c r="S25" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B26" s="79">
+      <c r="B26" s="35">
         <v>20</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="43"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="9"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -3429,28 +3573,28 @@
       <c r="M26" s="11"/>
       <c r="N26" s="18"/>
       <c r="O26" s="11"/>
-      <c r="P26" s="73" t="s">
+      <c r="P26" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="Q26" s="71" t="s">
+      <c r="Q26" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R26" s="71" t="s">
+      <c r="R26" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="S26" s="72" t="s">
+      <c r="S26" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B27" s="79">
+      <c r="B27" s="35">
         <v>21</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="9"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -3461,166 +3605,166 @@
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="18"/>
-      <c r="P27" s="73" t="s">
+      <c r="P27" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="71" t="s">
+      <c r="Q27" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R27" s="71" t="s">
+      <c r="R27" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="S27" s="72" t="s">
+      <c r="S27" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B28" s="83"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="38" t="s">
+      <c r="F28" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="79">
         <v>44655</v>
       </c>
-      <c r="I28" s="37">
+      <c r="I28" s="79">
         <v>44869</v>
       </c>
-      <c r="J28" s="67" t="s">
+      <c r="J28" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="67" t="s">
+      <c r="K28" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="L28" s="35">
+      <c r="L28" s="79">
         <v>44597</v>
       </c>
-      <c r="M28" s="35">
+      <c r="M28" s="79">
         <v>44809</v>
       </c>
-      <c r="N28" s="68" t="s">
+      <c r="N28" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="O28" s="41" t="s">
+      <c r="O28" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="P28" s="36" t="s">
+      <c r="P28" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="Q28" s="27" t="s">
+      <c r="Q28" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="R28" s="27" t="s">
+      <c r="R28" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="S28" s="30" t="s">
+      <c r="S28" s="73" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B29" s="84"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="85"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="28"/>
-      <c r="S29" s="31"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="82"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="82"/>
+      <c r="P29" s="71"/>
+      <c r="Q29" s="71"/>
+      <c r="R29" s="71"/>
+      <c r="S29" s="74"/>
     </row>
     <row r="30" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B30" s="84"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="85"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="28"/>
-      <c r="S30" s="31"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="82"/>
+      <c r="P30" s="71"/>
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
+      <c r="S30" s="74"/>
     </row>
     <row r="31" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B31" s="84"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="31"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="71"/>
+      <c r="S31" s="74"/>
     </row>
     <row r="32" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B32" s="84"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="85"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="28"/>
-      <c r="S32" s="31"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+      <c r="R32" s="71"/>
+      <c r="S32" s="74"/>
     </row>
     <row r="33" spans="2:19" ht="15" customHeight="1" thickBot="1">
-      <c r="B33" s="86"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="29"/>
-      <c r="S33" s="32"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="84"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="84"/>
+      <c r="M33" s="84"/>
+      <c r="N33" s="84"/>
+      <c r="O33" s="84"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="72"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="75"/>
     </row>
     <row r="34" spans="2:19" ht="14.25" customHeight="1"/>
     <row r="35" spans="2:19" ht="14.25" customHeight="1"/>
@@ -4554,17 +4698,24 @@
     <row r="963" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="B3:S4"/>
-    <mergeCell ref="F5:O5"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="P5:S6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="R28:R33"/>
+    <mergeCell ref="S28:S33"/>
+    <mergeCell ref="N28:N33"/>
+    <mergeCell ref="O28:O33"/>
+    <mergeCell ref="P28:P33"/>
+    <mergeCell ref="Q28:Q33"/>
+    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="F28:F33"/>
+    <mergeCell ref="G28:G33"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="H28:H33"/>
+    <mergeCell ref="I28:I33"/>
+    <mergeCell ref="J28:J33"/>
+    <mergeCell ref="K28:K33"/>
+    <mergeCell ref="L28:L33"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
@@ -4577,24 +4728,17 @@
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
-    <mergeCell ref="M28:M33"/>
-    <mergeCell ref="F28:F33"/>
-    <mergeCell ref="G28:G33"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="H28:H33"/>
-    <mergeCell ref="I28:I33"/>
-    <mergeCell ref="J28:J33"/>
-    <mergeCell ref="K28:K33"/>
-    <mergeCell ref="L28:L33"/>
-    <mergeCell ref="R28:R33"/>
-    <mergeCell ref="S28:S33"/>
-    <mergeCell ref="N28:N33"/>
-    <mergeCell ref="O28:O33"/>
-    <mergeCell ref="P28:P33"/>
-    <mergeCell ref="Q28:Q33"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="B3:S4"/>
+    <mergeCell ref="F5:O5"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="P5:S6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:O27">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
update pccv, project outline
</commit_message>
<xml_diff>
--- a/document/phan-cong-cong-viec.xlsx
+++ b/document/phan-cong-cong-viec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84367\Desktop\Đồ án chuyên nghành\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThanhTan\Documents\GitHub\super-tours-web-app\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>Project Leader:</t>
   </si>
@@ -104,45 +104,6 @@
     <t>Week 9</t>
   </si>
   <si>
-    <t xml:space="preserve">Sign up </t>
-  </si>
-  <si>
-    <t>CRUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit fileds </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pagination </t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forgot password </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reset password </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update password </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete user </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protect route </t>
-  </si>
-  <si>
-    <t>Authorization</t>
-  </si>
-  <si>
     <t>Render data inttemplate</t>
   </si>
   <si>
@@ -158,9 +119,6 @@
     <t>Văn Dũng</t>
   </si>
   <si>
-    <t>Update user info</t>
-  </si>
-  <si>
     <t>18/4/2022</t>
   </si>
   <si>
@@ -180,6 +138,81 @@
   </si>
   <si>
     <t>API docs</t>
+  </si>
+  <si>
+    <t>Tour API</t>
+  </si>
+  <si>
+    <t>1. CRUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Filter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Sort </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Limit fileds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Pagination </t>
+  </si>
+  <si>
+    <t>User API</t>
+  </si>
+  <si>
+    <t>1. Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Sign up </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Forgot password </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Reset password </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Update password </t>
+  </si>
+  <si>
+    <t>6. Update user info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Delete user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Protect route </t>
+  </si>
+  <si>
+    <t>9. Authorization</t>
+  </si>
+  <si>
+    <t>1. Base, header, footer</t>
+  </si>
+  <si>
+    <t>2. Account</t>
+  </si>
+  <si>
+    <t>3. Error</t>
+  </si>
+  <si>
+    <t>4. Login, sign up</t>
+  </si>
+  <si>
+    <t>5. Home page</t>
+  </si>
+  <si>
+    <t>6. Tour details</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>30/5/2022</t>
   </si>
 </sst>
 </file>
@@ -200,12 +233,14 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -218,44 +253,52 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF006411"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFDD0806"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -304,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -844,11 +887,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -913,7 +984,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -953,11 +1023,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
@@ -987,16 +1071,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1044,11 +1127,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1277,13 +1360,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1292,126 +1375,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7419975" y="1743075"/>
-          <a:ext cx="161925" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Oval 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8020050" y="1743075"/>
-          <a:ext cx="161925" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Oval 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1468,10 +1431,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Oval 22">
+        <xdr:cNvPr id="21" name="Oval 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1528,10 +1491,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Oval 23">
+        <xdr:cNvPr id="22" name="Oval 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1588,10 +1551,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Oval 24">
+        <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1648,10 +1611,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Oval 25">
+        <xdr:cNvPr id="24" name="Oval 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1708,10 +1671,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Oval 26">
+        <xdr:cNvPr id="25" name="Oval 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1755,23 +1718,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Oval 27">
+        <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1779,7 +1742,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7419975" y="2466975"/>
+          <a:off x="7419975" y="1743075"/>
           <a:ext cx="161925" cy="95250"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1815,23 +1778,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Oval 29">
+        <xdr:cNvPr id="27" name="Oval 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1839,7 +1802,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8582025" y="2647950"/>
+          <a:off x="8020050" y="1743075"/>
           <a:ext cx="161925" cy="95250"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1888,10 +1851,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Oval 31">
+        <xdr:cNvPr id="28" name="Oval 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1899,7 +1862,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8582025" y="2647950"/>
+          <a:off x="7419975" y="2466975"/>
           <a:ext cx="161925" cy="95250"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1948,10 +1911,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Oval 33">
+        <xdr:cNvPr id="30" name="Oval 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1995,23 +1958,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="Oval 36">
+        <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2019,67 +1982,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9182100" y="2647950"/>
-          <a:ext cx="161925" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Oval 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9182100" y="2647950"/>
+          <a:off x="8582025" y="2647950"/>
           <a:ext cx="161925" cy="95250"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2117,21 +2020,21 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Oval 39">
+        <xdr:cNvPr id="34" name="Oval 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2188,10 +2091,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Oval 40">
+        <xdr:cNvPr id="37" name="Oval 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2248,10 +2151,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="Oval 42">
+        <xdr:cNvPr id="39" name="Oval 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2260,6 +2163,66 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9182100" y="2647950"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Oval 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8582025" y="2647950"/>
           <a:ext cx="161925" cy="95250"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2308,6 +2271,126 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Oval 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="2647950"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Oval 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="2647950"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="45" name="Oval 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -2357,13 +2440,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2425,13 +2508,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2491,83 +2574,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Oval 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10868025" y="4657725"/>
-          <a:ext cx="161925" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2590,7 +2605,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln w="22225">
           <a:solidFill>
@@ -2629,13 +2644,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2689,13 +2704,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2717,6 +2732,414 @@
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Oval 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429750" y="5562600"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Oval 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429750" y="5743575"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Oval 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429750" y="5924550"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Oval 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9982200" y="6105525"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Oval 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9982200" y="6286500"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Oval 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9982200" y="6467475"/>
+          <a:ext cx="161925" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3011,10 +3434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S965"/>
+  <dimension ref="B1:T973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:E27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3025,20 +3448,20 @@
     <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="15" width="8.7109375" style="1" customWidth="1"/>
-    <col min="16" max="19" width="5.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="14.42578125" style="1"/>
+    <col min="7" max="16" width="8.7109375" style="1" customWidth="1"/>
+    <col min="17" max="20" width="5.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="G1" s="26"/>
+    <row r="1" spans="2:20" ht="14.25" customHeight="1" thickBot="1">
+      <c r="G1" s="25"/>
     </row>
-    <row r="2" spans="2:19" ht="21" customHeight="1" thickBot="1">
-      <c r="B2" s="64" t="s">
+    <row r="2" spans="2:20" ht="21" customHeight="1" thickBot="1">
+      <c r="B2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65"/>
+      <c r="C2" s="69"/>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3046,7 +3469,7 @@
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3055,128 +3478,137 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="68"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
     </row>
-    <row r="3" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B3" s="69" t="s">
+    <row r="3" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B3" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="72"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="76"/>
     </row>
-    <row r="4" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="75"/>
+    <row r="4" spans="2:20" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B4" s="77"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="79"/>
     </row>
-    <row r="5" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B5" s="78" t="s">
+    <row r="5" spans="2:20" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B5" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="76" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="78" t="s">
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="80"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="84"/>
     </row>
-    <row r="6" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B6" s="81"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="25" t="s">
+    <row r="6" spans="2:20" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B6" s="85"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="83"/>
+      <c r="O6" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="87"/>
     </row>
-    <row r="7" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B7" s="34">
+    <row r="7" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B7" s="33">
         <v>1</v>
       </c>
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="91"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -3187,28 +3619,29 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q7" s="28" t="s">
+      <c r="R7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="28" t="s">
+      <c r="S7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="29" t="s">
+      <c r="T7" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B8" s="35">
+    <row r="8" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B8" s="34">
         <v>2</v>
       </c>
-      <c r="C8" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
+      <c r="C8" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
@@ -3219,22 +3652,23 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="11"/>
+      <c r="Q8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="14"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="14"/>
     </row>
-    <row r="9" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B9" s="35">
+    <row r="9" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B9" s="34">
         <v>3</v>
       </c>
-      <c r="C9" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="60"/>
+      <c r="C9" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="9"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15"/>
@@ -3245,29 +3679,30 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="30" t="s">
+      <c r="P9" s="11"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="30" t="s">
+      <c r="S9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="31" t="s">
+      <c r="T9" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B10" s="35">
+    <row r="10" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B10" s="34">
         <v>4</v>
       </c>
-      <c r="C10" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="60"/>
+      <c r="C10" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="9"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -3275,22 +3710,19 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="14"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="30"/>
     </row>
-    <row r="11" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B11" s="35">
-        <v>5</v>
-      </c>
-      <c r="C11" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
+    <row r="11" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B11" s="34"/>
+      <c r="C11" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
       <c r="F11" s="9"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -3301,22 +3733,23 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="32" t="s">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="14"/>
+      <c r="R11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="13"/>
+      <c r="T11" s="14"/>
     </row>
-    <row r="12" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B12" s="35">
-        <v>6</v>
-      </c>
-      <c r="C12" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="60"/>
+    <row r="12" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B12" s="34"/>
+      <c r="C12" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="9"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -3327,22 +3760,23 @@
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="30" t="s">
+      <c r="P12" s="11"/>
+      <c r="Q12" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R12" s="13"/>
-      <c r="S12" s="14"/>
+      <c r="R12" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="13"/>
+      <c r="T12" s="14"/>
     </row>
-    <row r="13" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B13" s="35">
-        <v>7</v>
-      </c>
-      <c r="C13" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
+    <row r="13" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B13" s="34"/>
+      <c r="C13" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="9"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -3353,22 +3787,23 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="31" t="s">
+      <c r="P13" s="11"/>
+      <c r="Q13" s="31" t="s">
         <v>4</v>
       </c>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="T13" s="14"/>
     </row>
-    <row r="14" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B14" s="35">
-        <v>8</v>
-      </c>
-      <c r="C14" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="60"/>
+    <row r="14" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B14" s="34"/>
+      <c r="C14" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -3379,126 +3814,129 @@
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="30" t="s">
+      <c r="P14" s="11"/>
+      <c r="Q14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="30" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="15" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B15" s="35">
-        <v>9</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="60"/>
+    <row r="15" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B15" s="34"/>
+      <c r="C15" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="15"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="30" t="s">
+      <c r="P15" s="11"/>
+      <c r="Q15" s="31" t="s">
         <v>4</v>
       </c>
       <c r="R15" s="13"/>
-      <c r="S15" s="14"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="30" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="16" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B16" s="35">
-        <v>10</v>
-      </c>
-      <c r="C16" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
+    <row r="16" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B16" s="34">
+        <v>5</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="15"/>
+      <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="17"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="S16" s="14"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="14"/>
     </row>
-    <row r="17" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B17" s="35">
-        <v>11</v>
-      </c>
-      <c r="C17" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="60"/>
+    <row r="17" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B17" s="34"/>
+      <c r="C17" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="9"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="17"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="32" t="s">
+      <c r="P17" s="11"/>
+      <c r="Q17" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="14"/>
+      <c r="R17" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S17" s="13"/>
+      <c r="T17" s="14"/>
     </row>
-    <row r="18" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B18" s="35">
-        <v>12</v>
-      </c>
-      <c r="C18" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+    <row r="18" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B18" s="34"/>
+      <c r="C18" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="9"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="17"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="32" t="s">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
-      <c r="S18" s="14"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="30" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B19" s="35">
-        <v>13</v>
-      </c>
-      <c r="C19" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
+    <row r="19" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B19" s="34"/>
+      <c r="C19" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="9"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -3509,74 +3947,77 @@
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="30" t="s">
+      <c r="P19" s="11"/>
+      <c r="Q19" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="S19" s="14"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" s="14"/>
     </row>
-    <row r="20" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B20" s="35">
-        <v>14</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60"/>
+    <row r="20" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B20" s="34"/>
+      <c r="C20" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="9"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="18"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="11"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="30" t="s">
+      <c r="P20" s="11"/>
+      <c r="Q20" s="31" t="s">
         <v>4</v>
       </c>
       <c r="R20" s="13"/>
-      <c r="S20" s="14"/>
+      <c r="S20" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="T20" s="14"/>
     </row>
-    <row r="21" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B21" s="35">
-        <v>15</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
+    <row r="21" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B21" s="34"/>
+      <c r="C21" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="66"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="9"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="18"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="11"/>
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="31" t="s">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="31" t="s">
         <v>4</v>
       </c>
+      <c r="R21" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S21" s="29"/>
+      <c r="T21" s="14"/>
     </row>
-    <row r="22" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B22" s="35">
-        <v>16</v>
-      </c>
-      <c r="C22" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60"/>
+    <row r="22" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B22" s="34"/>
+      <c r="C22" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
       <c r="F22" s="9"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -3587,22 +4028,23 @@
       <c r="M22" s="18"/>
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
-      <c r="P22" s="32" t="s">
+      <c r="P22" s="11"/>
+      <c r="Q22" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="14"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="30" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B23" s="35">
-        <v>17</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="60"/>
+    <row r="23" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B23" s="34"/>
+      <c r="C23" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="66"/>
+      <c r="E23" s="67"/>
       <c r="F23" s="9"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3610,25 +4052,26 @@
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="11"/>
       <c r="O23" s="11"/>
-      <c r="P23" s="32" t="s">
+      <c r="P23" s="11"/>
+      <c r="Q23" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="14"/>
+      <c r="R23" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S23" s="13"/>
+      <c r="T23" s="30"/>
     </row>
-    <row r="24" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B24" s="35">
-        <v>18</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
+    <row r="24" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B24" s="34"/>
+      <c r="C24" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="66"/>
+      <c r="E24" s="67"/>
       <c r="F24" s="9"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -3636,25 +4079,26 @@
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="11"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="32" t="s">
+      <c r="P24" s="11"/>
+      <c r="Q24" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="14"/>
+      <c r="R24" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S24" s="13"/>
+      <c r="T24" s="14"/>
     </row>
-    <row r="25" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B25" s="35">
-        <v>19</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="42"/>
+    <row r="25" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B25" s="34"/>
+      <c r="C25" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="66"/>
+      <c r="E25" s="67"/>
       <c r="F25" s="9"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -3664,23 +4108,26 @@
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="18"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="32" t="s">
+      <c r="O25" s="18"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
-      <c r="S25" s="14"/>
+      <c r="S25" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="T25" s="14"/>
     </row>
-    <row r="26" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B26" s="35">
-        <v>20</v>
-      </c>
-      <c r="C26" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="60"/>
+    <row r="26" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B26" s="34">
+        <v>6</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="9"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -3690,29 +4137,26 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
       <c r="N26" s="18"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="32" t="s">
+      <c r="O26" s="18"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q26" s="30" t="s">
+      <c r="R26" s="13"/>
+      <c r="S26" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R26" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="S26" s="31" t="s">
-        <v>5</v>
-      </c>
+      <c r="T26" s="14"/>
     </row>
-    <row r="27" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B27" s="35">
-        <v>21</v>
-      </c>
-      <c r="C27" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
+    <row r="27" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B27" s="34">
+        <v>7</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="41"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="9"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -3722,61 +4166,59 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
       <c r="N27" s="18"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="32" t="s">
+      <c r="O27" s="18"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="30" t="s">
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R27" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="S27" s="31" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="28" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B28" s="35">
-        <v>22</v>
-      </c>
-      <c r="C28" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="60"/>
+    <row r="28" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B28" s="34">
+        <v>8</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
       <c r="F28" s="9"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
-      <c r="I28" s="16"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
       <c r="N28" s="18"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="32" t="s">
+      <c r="O28" s="18"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q28" s="30" t="s">
+      <c r="R28" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R28" s="30" t="s">
+      <c r="S28" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="S28" s="31" t="s">
+      <c r="T28" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B29" s="35">
-        <v>23</v>
-      </c>
-      <c r="C29" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="63"/>
+    <row r="29" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B29" s="34">
+        <v>9</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="61"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="9"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -3785,182 +4227,403 @@
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
+      <c r="N29" s="18"/>
       <c r="O29" s="18"/>
-      <c r="P29" s="32" t="s">
+      <c r="P29" s="11"/>
+      <c r="Q29" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q29" s="30" t="s">
+      <c r="R29" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R29" s="30" t="s">
+      <c r="S29" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="S29" s="31" t="s">
+      <c r="T29" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B30" s="36"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="55" t="s">
+    <row r="30" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B30" s="34">
+        <v>10</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="61"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="30"/>
+    </row>
+    <row r="31" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B31" s="34"/>
+      <c r="C31" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="44"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R31" s="29"/>
+      <c r="S31" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="T31" s="30"/>
+    </row>
+    <row r="32" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B32" s="34"/>
+      <c r="C32" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R32" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S32" s="29"/>
+      <c r="T32" s="30"/>
+    </row>
+    <row r="33" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B33" s="34"/>
+      <c r="C33" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R33" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S33" s="29"/>
+      <c r="T33" s="30"/>
+    </row>
+    <row r="34" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B34" s="34"/>
+      <c r="C34" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="T34" s="30"/>
+    </row>
+    <row r="35" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B35" s="34"/>
+      <c r="C35" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="44"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
+      <c r="T35" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B36" s="34"/>
+      <c r="C36" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B37" s="34">
+        <v>11</v>
+      </c>
+      <c r="C37" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="64"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R37" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S37" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="T37" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B38" s="35"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="52" t="s">
+      <c r="G38" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H38" s="57">
         <v>44655</v>
       </c>
-      <c r="I30" s="54">
+      <c r="I38" s="57">
         <v>44662</v>
       </c>
-      <c r="J30" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="K30" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="L30" s="54">
+      <c r="J38" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="K38" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="L38" s="57">
         <v>44683</v>
       </c>
-      <c r="M30" s="54">
+      <c r="M38" s="57">
         <v>44690</v>
       </c>
-      <c r="N30" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="O30" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="P30" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q30" s="43" t="s">
+      <c r="N38" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="P38" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q38" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="R38" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="R30" s="43" t="s">
+      <c r="S38" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="S30" s="46" t="s">
-        <v>43</v>
+      <c r="T38" s="49" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
-      <c r="S31" s="47"/>
+    <row r="39" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B39" s="36"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="47"/>
+      <c r="R39" s="47"/>
+      <c r="S39" s="47"/>
+      <c r="T39" s="50"/>
     </row>
-    <row r="32" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="44"/>
-      <c r="S32" s="47"/>
+    <row r="40" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="47"/>
+      <c r="R40" s="47"/>
+      <c r="S40" s="47"/>
+      <c r="T40" s="50"/>
     </row>
-    <row r="33" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="47"/>
+    <row r="41" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="47"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="47"/>
+      <c r="T41" s="50"/>
     </row>
-    <row r="34" spans="2:19" ht="14.25" customHeight="1">
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="44"/>
-      <c r="Q34" s="44"/>
-      <c r="R34" s="44"/>
-      <c r="S34" s="47"/>
+    <row r="42" spans="2:20" ht="14.25" customHeight="1">
+      <c r="B42" s="36"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="47"/>
+      <c r="T42" s="50"/>
     </row>
-    <row r="35" spans="2:19" ht="15" customHeight="1" thickBot="1">
-      <c r="B35" s="39"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="45"/>
-      <c r="Q35" s="45"/>
-      <c r="R35" s="45"/>
-      <c r="S35" s="48"/>
+    <row r="43" spans="2:20" ht="15" customHeight="1" thickBot="1">
+      <c r="B43" s="38"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="54"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="54"/>
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="51"/>
     </row>
-    <row r="36" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="37" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="38" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="39" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="40" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="41" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="42" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="43" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="44" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="45" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="46" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="47" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="48" spans="2:19" ht="14.25" customHeight="1"/>
+    <row r="44" spans="2:20" ht="14.25" customHeight="1"/>
+    <row r="45" spans="2:20" ht="14.25" customHeight="1"/>
+    <row r="46" spans="2:20" ht="14.25" customHeight="1"/>
+    <row r="47" spans="2:20" ht="14.25" customHeight="1"/>
+    <row r="48" spans="2:20" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -4878,61 +5541,80 @@
     <row r="963" ht="14.25" customHeight="1"/>
     <row r="964" ht="14.25" customHeight="1"/>
     <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="C11:E11"/>
+  <mergeCells count="52">
+    <mergeCell ref="C12:E12"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="B3:S4"/>
-    <mergeCell ref="F5:O5"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="B3:T4"/>
+    <mergeCell ref="F5:P5"/>
     <mergeCell ref="B5:E6"/>
-    <mergeCell ref="P5:S6"/>
+    <mergeCell ref="Q5:T6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
-    <mergeCell ref="M30:M35"/>
-    <mergeCell ref="F30:F35"/>
-    <mergeCell ref="G30:G35"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="M38:M43"/>
+    <mergeCell ref="F38:F43"/>
+    <mergeCell ref="G38:G43"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="H38:H43"/>
+    <mergeCell ref="I38:I43"/>
+    <mergeCell ref="J38:J43"/>
+    <mergeCell ref="K38:K43"/>
+    <mergeCell ref="L38:L43"/>
+    <mergeCell ref="S38:S43"/>
+    <mergeCell ref="T38:T43"/>
+    <mergeCell ref="N38:N43"/>
+    <mergeCell ref="P38:P43"/>
+    <mergeCell ref="Q38:Q43"/>
+    <mergeCell ref="R38:R43"/>
+    <mergeCell ref="O38:O43"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="H30:H35"/>
-    <mergeCell ref="I30:I35"/>
-    <mergeCell ref="J30:J35"/>
-    <mergeCell ref="K30:K35"/>
-    <mergeCell ref="L30:L35"/>
-    <mergeCell ref="R30:R35"/>
-    <mergeCell ref="S30:S35"/>
-    <mergeCell ref="N30:N35"/>
-    <mergeCell ref="O30:O35"/>
-    <mergeCell ref="P30:P35"/>
-    <mergeCell ref="Q30:Q35"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C32:E32"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7:O29">
+  <conditionalFormatting sqref="F7:P37">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:O29">
+  <conditionalFormatting sqref="F7:P37">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:O29">
+  <conditionalFormatting sqref="F7:P37">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>

</xml_diff>